<commit_message>
feat: add initial HTML report for LPU validation with statistics and summaries
</commit_message>
<xml_diff>
--- a/outputs/validacao_lpu.xlsx
+++ b/outputs/validacao_lpu.xlsx
@@ -2543,7 +2543,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Para ressarcimento</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -6369,7 +6369,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6402,17 +6402,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Para ressarcimento</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>166062.14</v>
+        <v>364.18</v>
       </c>
       <c r="D2" t="n">
-        <v>770388.67</v>
+        <v>54183.25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Para ressarcimento</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>76</v>
+      </c>
+      <c r="C3" t="n">
+        <v>165697.96</v>
+      </c>
+      <c r="D3" t="n">
+        <v>716205.42</v>
       </c>
     </row>
   </sheetData>
@@ -6426,7 +6442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6518,20 +6534,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Para ressarcimento</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>31559.19</v>
+        <v>364.18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Forros e Divisórias</t>
+          <t>Fachada e Comunicação Visual</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -6540,16 +6556,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>15477.78</v>
+        <v>31195.01</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Instalações Elétricas</t>
+          <t>Forros e Divisórias</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -6558,16 +6574,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>15120.5</v>
+        <v>15477.78</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Instalações Hidráulicas</t>
+          <t>Instalações Elétricas</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -6579,13 +6595,13 @@
         <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>6853.04</v>
+        <v>15120.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Limpeza Final</t>
+          <t>Instalações Hidráulicas</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -6594,16 +6610,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>4781.04</v>
+        <v>6853.04</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mobiliário</t>
+          <t>Limpeza Final</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -6612,16 +6628,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D10" t="n">
-        <v>21402.5</v>
+        <v>4781.04</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Pintura</t>
+          <t>Mobiliário</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -6630,16 +6646,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D11" t="n">
-        <v>8687.940000000001</v>
+        <v>21402.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Pisos</t>
+          <t>Pintura</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -6648,16 +6664,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" t="n">
-        <v>19163.86</v>
+        <v>8687.940000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Revestimentos e Acabamentos</t>
+          <t>Pisos</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -6669,24 +6685,42 @@
         <v>5</v>
       </c>
       <c r="D13" t="n">
-        <v>9201.950000000001</v>
+        <v>19163.86</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Revestimentos e Acabamentos</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Para ressarcimento</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>9201.950000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>Segurança e Automação</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Para ressarcimento</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Para ressarcimento</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
         <v>8</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>9028</v>
       </c>
     </row>
@@ -6701,7 +6735,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6847,20 +6881,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Para ressarcimento</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>31559.19</v>
+        <v>364.18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>UPE_00008</t>
+          <t>UPE_00007</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -6869,16 +6903,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
-        <v>6853.04</v>
+        <v>31195.01</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>UPE_00009</t>
+          <t>UPE_00008</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -6890,13 +6924,13 @@
         <v>10</v>
       </c>
       <c r="D10" t="n">
-        <v>15120.5</v>
+        <v>6853.04</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UPE_00010</t>
+          <t>UPE_00009</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -6905,16 +6939,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>11026</v>
+        <v>15120.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UPE_00011</t>
+          <t>UPE_00010</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -6923,16 +6957,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D12" t="n">
-        <v>9028</v>
+        <v>11026</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>UPE_00012</t>
+          <t>UPE_00011</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -6944,24 +6978,42 @@
         <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>21402.5</v>
+        <v>9028</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>UPE_00012</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Para ressarcimento</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" t="n">
+        <v>21402.5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>UPE_00013</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Para ressarcimento</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Para ressarcimento</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
         <v>3</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>4781.04</v>
       </c>
     </row>

</xml_diff>